<commit_message>
Paper and Excel Done
</commit_message>
<xml_diff>
--- a/TermProjectReport/TermProject ExcelGraph.xlsx
+++ b/TermProjectReport/TermProject ExcelGraph.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="9900" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="-460" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Bubble Sort Data(milliseconds)</t>
   </si>
@@ -37,18 +37,28 @@
   <si>
     <t>Bubble Sort vs Selection Sort</t>
   </si>
+  <si>
+    <t># of Times</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -60,7 +70,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -83,16 +93,40 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -138,7 +172,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -152,7 +185,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$C$2</c:f>
+              <c:f>Data!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -166,7 +199,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$B$2:$B$11</c:f>
+              <c:f>Data!$C$2:$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -204,7 +237,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$3:$C$11</c:f>
+              <c:f>Data!$D$3:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -245,7 +278,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$D$2</c:f>
+              <c:f>Data!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -259,7 +292,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$B$2:$B$11</c:f>
+              <c:f>Data!$C$2:$C$11</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -297,7 +330,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$3:$D$11</c:f>
+              <c:f>Data!$E$3:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -343,11 +376,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2111066472"/>
-        <c:axId val="-2111063496"/>
+        <c:axId val="-2119384440"/>
+        <c:axId val="-2119202120"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2111066472"/>
+        <c:axId val="-2119384440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -356,7 +389,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111063496"/>
+        <c:crossAx val="-2119202120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -364,7 +397,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111063496"/>
+        <c:axId val="-2119202120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -393,21 +426,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111066472"/>
+        <c:crossAx val="-2119384440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -462,7 +493,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -476,7 +506,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$C$2</c:f>
+              <c:f>Data!$D$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -490,7 +520,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$11</c:f>
+              <c:f>Data!$B$2:$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -528,7 +558,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$C$3:$C$11</c:f>
+              <c:f>Data!$D$3:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -569,7 +599,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$D$2</c:f>
+              <c:f>Data!$E$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -583,7 +613,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$A$2:$A$11</c:f>
+              <c:f>Data!$B$2:$B$11</c:f>
               <c:strCache>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
@@ -621,7 +651,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$D$3:$D$11</c:f>
+              <c:f>Data!$E$3:$E$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
@@ -667,11 +697,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2110982344"/>
-        <c:axId val="-2110979368"/>
+        <c:axId val="-2119206872"/>
+        <c:axId val="-2119451176"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2110982344"/>
+        <c:axId val="-2119206872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +710,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110979368"/>
+        <c:crossAx val="-2119451176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -688,7 +718,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110979368"/>
+        <c:axId val="-2119451176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -717,21 +747,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110982344"/>
+        <c:crossAx val="-2119206872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1142,171 +1170,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:5">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="4"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" s="2">
+    <row r="3" spans="1:5">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1">
         <v>50</v>
       </c>
-      <c r="B3" s="2">
+      <c r="C3" s="1">
         <v>100</v>
       </c>
-      <c r="C3" s="2">
+      <c r="D3" s="1">
         <v>7</v>
       </c>
-      <c r="D3" s="2">
+      <c r="E3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" s="2">
+    <row r="4" spans="1:5">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="1">
         <v>50</v>
       </c>
-      <c r="B4" s="2">
+      <c r="C4" s="1">
         <v>1000</v>
       </c>
-      <c r="C4" s="2">
+      <c r="D4" s="1">
         <v>9</v>
       </c>
-      <c r="D4" s="2">
+      <c r="E4" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" s="2">
+    <row r="5" spans="1:5">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
         <v>50</v>
       </c>
-      <c r="B5" s="2">
+      <c r="C5" s="1">
         <v>10000</v>
       </c>
-      <c r="C5" s="2">
+      <c r="D5" s="1">
         <v>62</v>
       </c>
-      <c r="D5" s="2">
+      <c r="E5" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2">
+    <row r="6" spans="1:5">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1">
         <v>250</v>
       </c>
-      <c r="B6" s="2">
+      <c r="C6" s="1">
         <v>100</v>
       </c>
-      <c r="C6" s="2">
+      <c r="D6" s="1">
         <v>10</v>
       </c>
-      <c r="D6" s="2">
+      <c r="E6" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="2">
+    <row r="7" spans="1:5">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="1">
         <v>250</v>
       </c>
-      <c r="B7" s="2">
+      <c r="C7" s="1">
         <v>1000</v>
       </c>
-      <c r="C7" s="2">
+      <c r="D7" s="1">
         <v>137</v>
       </c>
-      <c r="D7" s="2">
+      <c r="E7" s="1">
         <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="2">
+    <row r="8" spans="1:5">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1">
         <v>250</v>
       </c>
-      <c r="B8" s="2">
+      <c r="C8" s="1">
         <v>10000</v>
       </c>
-      <c r="C8" s="2">
+      <c r="D8" s="1">
         <v>830</v>
       </c>
-      <c r="D8" s="2">
+      <c r="E8" s="1">
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="2">
+    <row r="9" spans="1:5">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="1">
         <v>500</v>
       </c>
-      <c r="B9" s="2">
+      <c r="C9" s="1">
         <v>100</v>
       </c>
-      <c r="C9" s="2">
+      <c r="D9" s="1">
         <v>25</v>
       </c>
-      <c r="D9" s="2">
+      <c r="E9" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="2">
+    <row r="10" spans="1:5">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="1">
         <v>500</v>
       </c>
-      <c r="B10" s="2">
+      <c r="C10" s="1">
         <v>1000</v>
       </c>
-      <c r="C10" s="2">
+      <c r="D10" s="1">
         <v>248</v>
       </c>
-      <c r="D10" s="2">
+      <c r="E10" s="1">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="2">
+    <row r="11" spans="1:5">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="1">
         <v>500</v>
       </c>
-      <c r="B11" s="2">
+      <c r="C11" s="1">
         <v>10000</v>
       </c>
-      <c r="C11" s="2">
+      <c r="D11" s="1">
         <v>2426</v>
       </c>
-      <c r="D11" s="2">
+      <c r="E11" s="1">
         <v>654</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>